<commit_message>
add more to code outline
</commit_message>
<xml_diff>
--- a/Chapter4/chinook_data.xlsx
+++ b/Chapter4/chinook_data.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\words\github\Practical-Data-Science-with-Python\Chapter4\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A5E1FD-B69D-4BEB-938A-673AA923A994}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="sales_data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -115,8 +121,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,6 +185,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -225,7 +239,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -257,9 +271,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -291,6 +323,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -466,14 +516,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -484,7 +534,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>1561.23</v>
       </c>
@@ -495,7 +545,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>185.13</v>
       </c>
@@ -506,9 +556,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
-        <v>502.9200000000001</v>
+        <v>502.92000000000007</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -517,9 +567,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
-        <v>466.2900000000002</v>
+        <v>466.29000000000019</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -528,7 +578,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>13.86</v>
       </c>
@@ -539,7 +589,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>112.86</v>
       </c>
@@ -550,7 +600,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>789.0300000000002</v>
       </c>
@@ -561,7 +611,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>58.41</v>
       </c>
@@ -572,7 +622,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>13.86</v>
       </c>
@@ -583,9 +633,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
-        <v>45.53999999999999</v>
+        <v>45.539999999999992</v>
       </c>
       <c r="B11" t="s">
         <v>3</v>
@@ -594,7 +644,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>13.86</v>
       </c>
@@ -605,7 +655,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>41.58</v>
       </c>
@@ -616,9 +666,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
-        <v>50.48999999999999</v>
+        <v>50.489999999999988</v>
       </c>
       <c r="B14" t="s">
         <v>3</v>
@@ -627,7 +677,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>69.3</v>
       </c>
@@ -638,7 +688,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>17.82</v>
       </c>
@@ -649,7 +699,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>41.58</v>
       </c>
@@ -660,7 +710,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>27.72</v>
       </c>
@@ -671,9 +721,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
-        <v>1364.770000000001</v>
+        <v>1364.7700000000009</v>
       </c>
       <c r="B19" t="s">
         <v>4</v>
@@ -682,7 +732,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>173.25</v>
       </c>
@@ -693,9 +743,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
-        <v>488.2300000000002</v>
+        <v>488.23000000000019</v>
       </c>
       <c r="B21" t="s">
         <v>4</v>
@@ -704,9 +754,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
-        <v>264.3799999999999</v>
+        <v>264.37999999999988</v>
       </c>
       <c r="B22" t="s">
         <v>4</v>
@@ -715,7 +765,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <v>27.72</v>
       </c>
@@ -726,7 +776,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <v>44.55</v>
       </c>
@@ -737,9 +787,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
-        <v>804.1400000000006</v>
+        <v>804.14000000000055</v>
       </c>
       <c r="B25" t="s">
         <v>4</v>
@@ -748,7 +798,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A26">
         <v>58.41</v>
       </c>
@@ -759,7 +809,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A27">
         <v>61.38</v>
       </c>
@@ -770,7 +820,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A28">
         <v>55.44</v>
       </c>
@@ -781,7 +831,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A29">
         <v>27.72</v>
       </c>
@@ -792,7 +842,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A30">
         <v>27.72</v>
       </c>
@@ -803,7 +853,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A31">
         <v>41.58</v>
       </c>
@@ -814,7 +864,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A32">
         <v>103.99</v>
       </c>
@@ -825,7 +875,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A33">
         <v>38.64</v>
       </c>
@@ -836,7 +886,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A34">
         <v>41.58</v>
       </c>
@@ -847,7 +897,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A35">
         <v>29.73</v>
       </c>
@@ -858,7 +908,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A36">
         <v>35.82</v>
       </c>
@@ -869,7 +919,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A37">
         <v>225.48</v>
       </c>
@@ -880,9 +930,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A38">
-        <v>49.71999999999999</v>
+        <v>49.719999999999992</v>
       </c>
       <c r="B38" t="s">
         <v>4</v>
@@ -891,9 +941,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A39">
-        <v>148.11</v>
+        <v>148.11000000000001</v>
       </c>
       <c r="B39" t="s">
         <v>4</v>
@@ -902,7 +952,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A40">
         <v>37.72</v>
       </c>
@@ -913,9 +963,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A41">
-        <v>80.28999999999999</v>
+        <v>80.289999999999992</v>
       </c>
       <c r="B41" t="s">
         <v>4</v>
@@ -924,9 +974,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A42">
-        <v>99.07999999999998</v>
+        <v>99.079999999999984</v>
       </c>
       <c r="B42" t="s">
         <v>4</v>
@@ -935,7 +985,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A43">
         <v>1586.62</v>
       </c>
@@ -946,9 +996,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A44">
-        <v>153.45</v>
+        <v>153.44999999999999</v>
       </c>
       <c r="B44" t="s">
         <v>5</v>
@@ -957,7 +1007,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A45">
         <v>177.26</v>
       </c>
@@ -968,9 +1018,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A46">
-        <v>437.7600000000003</v>
+        <v>437.76000000000028</v>
       </c>
       <c r="B46" t="s">
         <v>5</v>
@@ -979,7 +1029,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A47">
         <v>13.86</v>
       </c>
@@ -990,7 +1040,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A48">
         <v>105.93</v>
       </c>
@@ -1001,9 +1051,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A49">
-        <v>613.0600000000006</v>
+        <v>613.06000000000063</v>
       </c>
       <c r="B49" t="s">
         <v>5</v>
@@ -1012,7 +1062,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A50">
         <v>100.98</v>
       </c>
@@ -1023,7 +1073,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A51">
         <v>78.3</v>
       </c>
@@ -1034,7 +1084,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A52">
         <v>54.45</v>
       </c>
@@ -1045,7 +1095,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A53">
         <v>20.79</v>
       </c>
@@ -1056,7 +1106,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A54">
         <v>41.58</v>
       </c>
@@ -1067,9 +1117,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A55">
-        <v>16.83</v>
+        <v>16.829999999999998</v>
       </c>
       <c r="B55" t="s">
         <v>5</v>
@@ -1078,7 +1128,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A56">
         <v>31.72</v>
       </c>
@@ -1089,7 +1139,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A57">
         <v>15.86</v>
       </c>
@@ -1100,9 +1150,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A58">
-        <v>40.59</v>
+        <v>40.590000000000003</v>
       </c>
       <c r="B58" t="s">
         <v>5</v>
@@ -1111,7 +1161,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A59">
         <v>29.82</v>
       </c>
@@ -1122,9 +1172,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A60">
-        <v>273.1900000000001</v>
+        <v>273.19000000000011</v>
       </c>
       <c r="B60" t="s">
         <v>5</v>
@@ -1133,7 +1183,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A61">
         <v>66.61999999999999</v>
       </c>
@@ -1144,9 +1194,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A62">
-        <v>73.45999999999999</v>
+        <v>73.459999999999994</v>
       </c>
       <c r="B62" t="s">
         <v>5</v>
@@ -1155,7 +1205,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A63">
         <v>18.86</v>
       </c>
@@ -1166,7 +1216,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A64">
         <v>63.44</v>
       </c>
@@ -1177,7 +1227,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A65">
         <v>111.97</v>
       </c>
@@ -1188,9 +1238,9 @@
         <v>31</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A66">
-        <v>1536.160000000002</v>
+        <v>1536.1600000000019</v>
       </c>
       <c r="B66" t="s">
         <v>6</v>
@@ -1199,9 +1249,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A67">
-        <v>67.31999999999999</v>
+        <v>67.319999999999993</v>
       </c>
       <c r="B67" t="s">
         <v>6</v>
@@ -1210,9 +1260,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A68">
-        <v>487.1400000000003</v>
+        <v>487.14000000000033</v>
       </c>
       <c r="B68" t="s">
         <v>6</v>
@@ -1221,9 +1271,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A69">
-        <v>345.6300000000001</v>
+        <v>345.63000000000011</v>
       </c>
       <c r="B69" t="s">
         <v>6</v>
@@ -1232,7 +1282,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A70">
         <v>27.72</v>
       </c>
@@ -1243,9 +1293,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A71">
-        <v>73.25999999999999</v>
+        <v>73.259999999999991</v>
       </c>
       <c r="B71" t="s">
         <v>6</v>
@@ -1254,9 +1304,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A72">
-        <v>543.6200000000006</v>
+        <v>543.62000000000057</v>
       </c>
       <c r="B72" t="s">
         <v>6</v>
@@ -1265,9 +1315,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A73">
-        <v>73.25999999999999</v>
+        <v>73.259999999999991</v>
       </c>
       <c r="B73" t="s">
         <v>6</v>
@@ -1276,9 +1326,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A74">
-        <v>86.20999999999999</v>
+        <v>86.21</v>
       </c>
       <c r="B74" t="s">
         <v>6</v>
@@ -1287,7 +1337,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A75">
         <v>45.54</v>
       </c>
@@ -1298,7 +1348,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A76">
         <v>41.58</v>
       </c>
@@ -1309,9 +1359,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A77">
-        <v>99.98999999999999</v>
+        <v>99.99</v>
       </c>
       <c r="B77" t="s">
         <v>6</v>
@@ -1320,7 +1370,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A78">
         <v>47.58</v>
       </c>
@@ -1331,7 +1381,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A79">
         <v>41.58</v>
       </c>
@@ -1342,7 +1392,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A80">
         <v>61.44</v>
       </c>
@@ -1353,7 +1403,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A81">
         <v>10.91</v>
       </c>
@@ -1364,9 +1414,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A82">
-        <v>161.89</v>
+        <v>161.88999999999999</v>
       </c>
       <c r="B82" t="s">
         <v>6</v>
@@ -1375,9 +1425,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A83">
-        <v>82.52999999999999</v>
+        <v>82.529999999999987</v>
       </c>
       <c r="B83" t="s">
         <v>6</v>
@@ -1386,7 +1436,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A84">
         <v>193.74</v>
       </c>
@@ -1397,7 +1447,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A85">
         <v>55.72</v>
       </c>
@@ -1408,7 +1458,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A86">
         <v>67.44</v>
       </c>
@@ -1419,7 +1469,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="87" spans="1:3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A87">
         <v>105.99</v>
       </c>
@@ -1430,9 +1480,9 @@
         <v>31</v>
       </c>
     </row>
-    <row r="88" spans="1:3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A88">
-        <v>1671.240000000001</v>
+        <v>1671.2400000000009</v>
       </c>
       <c r="B88" t="s">
         <v>7</v>
@@ -1441,9 +1491,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A89">
-        <v>167.3099999999999</v>
+        <v>167.30999999999989</v>
       </c>
       <c r="B89" t="s">
         <v>7</v>
@@ -1452,9 +1502,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A90">
-        <v>437.5800000000003</v>
+        <v>437.58000000000033</v>
       </c>
       <c r="B90" t="s">
         <v>7</v>
@@ -1463,9 +1513,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A91">
-        <v>447.6000000000002</v>
+        <v>447.60000000000019</v>
       </c>
       <c r="B91" t="s">
         <v>7</v>
@@ -1474,9 +1524,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A92">
-        <v>93.05999999999999</v>
+        <v>93.059999999999988</v>
       </c>
       <c r="B92" t="s">
         <v>7</v>
@@ -1485,9 +1535,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="93" spans="1:3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A93">
-        <v>722.7000000000004</v>
+        <v>722.70000000000039</v>
       </c>
       <c r="B93" t="s">
         <v>7</v>
@@ -1496,7 +1546,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="94" spans="1:3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A94">
         <v>41.58</v>
       </c>
@@ -1507,7 +1557,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="1:3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A95">
         <v>41.58</v>
       </c>
@@ -1518,7 +1568,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="96" spans="1:3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A96">
         <v>23.76</v>
       </c>
@@ -1529,7 +1579,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="97" spans="1:3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A97">
         <v>27.72</v>
       </c>
@@ -1540,7 +1590,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="98" spans="1:3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A98">
         <v>27.72</v>
       </c>
@@ -1551,9 +1601,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="99" spans="1:3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A99">
-        <v>48.50999999999999</v>
+        <v>48.509999999999991</v>
       </c>
       <c r="B99" t="s">
         <v>7</v>
@@ -1562,7 +1612,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="100" spans="1:3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A100">
         <v>13.86</v>
       </c>
@@ -1573,7 +1623,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="101" spans="1:3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A101">
         <v>41.58</v>
       </c>
@@ -1584,7 +1634,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="102" spans="1:3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A102">
         <v>6.93</v>
       </c>
@@ -1595,7 +1645,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="103" spans="1:3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A103">
         <v>25.86</v>
       </c>
@@ -1606,7 +1656,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="104" spans="1:3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A104">
         <v>157.15</v>
       </c>
@@ -1617,9 +1667,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="105" spans="1:3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A105">
-        <v>129.3</v>
+        <v>129.30000000000001</v>
       </c>
       <c r="B105" t="s">
         <v>7</v>

</xml_diff>